<commit_message>
Commit Exception and Dto
</commit_message>
<xml_diff>
--- a/datarsapi.xlsx
+++ b/datarsapi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dimitra\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dimitra\Desktop\AllProjects\DCompany\rsapi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A92EFC-D5A7-4B91-9683-24FBCC683A28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156C0C49-B2D5-4C71-BD28-C828C1D50DCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="72">
   <si>
     <t>Creativity</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>Junior</t>
+  </si>
+  <si>
+    <t>ApplicationDate</t>
   </si>
 </sst>
 </file>
@@ -289,9 +292,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
@@ -606,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,15 +621,16 @@
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -636,16 +641,16 @@
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>20</v>
@@ -653,8 +658,11 @@
       <c r="I1" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -664,26 +672,29 @@
       <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
-        <v>31</v>
+      <c r="D2" s="2">
+        <v>43983</v>
       </c>
       <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
         <v>30</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>70</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -693,26 +704,29 @@
       <c r="C3" t="s">
         <v>34</v>
       </c>
-      <c r="D3" t="s">
-        <v>31</v>
+      <c r="D3" s="2">
+        <v>43984</v>
       </c>
       <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>70</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>3</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -722,26 +736,29 @@
       <c r="C4" t="s">
         <v>41</v>
       </c>
-      <c r="D4" t="s">
-        <v>31</v>
+      <c r="D4" s="2">
+        <v>43984</v>
       </c>
       <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
         <v>29</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>70</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -751,26 +768,29 @@
       <c r="C5" t="s">
         <v>62</v>
       </c>
-      <c r="D5" t="s">
-        <v>31</v>
+      <c r="D5" s="2">
+        <v>43983</v>
       </c>
       <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
         <v>29</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>40</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>63</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>23</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -780,26 +800,29 @@
       <c r="C6" t="s">
         <v>44</v>
       </c>
-      <c r="D6" t="s">
-        <v>31</v>
+      <c r="D6" s="2">
+        <v>43987</v>
       </c>
       <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
         <v>29</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>39</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>6</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>3</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -809,26 +832,29 @@
       <c r="C7" t="s">
         <v>47</v>
       </c>
-      <c r="D7" t="s">
-        <v>31</v>
+      <c r="D7" s="2">
+        <v>43987</v>
       </c>
       <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
         <v>29</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>40</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>6</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>3</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -838,26 +864,29 @@
       <c r="C8" t="s">
         <v>50</v>
       </c>
-      <c r="D8" t="s">
-        <v>31</v>
+      <c r="D8" s="2">
+        <v>43992</v>
       </c>
       <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>39</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>55</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>23</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -867,26 +896,29 @@
       <c r="C9" t="s">
         <v>53</v>
       </c>
-      <c r="D9" t="s">
-        <v>31</v>
+      <c r="D9" s="2">
+        <v>43993</v>
       </c>
       <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
         <v>29</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>39</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>54</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>55</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -896,22 +928,25 @@
       <c r="C10" t="s">
         <v>58</v>
       </c>
-      <c r="D10" t="s">
-        <v>31</v>
+      <c r="D10" s="2">
+        <v>43993</v>
       </c>
       <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
         <v>29</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>39</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>59</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>55</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>